<commit_message>
Inserindo artefato 1 para a correção da AC5
Ajustes da classificação do evento número 4 de " Não Evento" para "Extemporâneo";
Ajuste do nome do evento número 6 de "Atendente recebe Validação" para "Cliente envia validação";
Ajuste da classificação do evento número 12 e 13 de "Externo - Não Previsível" para "Externo - Previsível".
</commit_message>
<xml_diff>
--- a/17 - Análise dos Eventos para cada Cenário.xlsx
+++ b/17 - Análise dos Eventos para cada Cenário.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13\Desktop\AC 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -104,9 +104,6 @@
     <t>Técnico realiza visita</t>
   </si>
   <si>
-    <t>Atendente recebe validação</t>
-  </si>
-  <si>
     <t>x(6)</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>x(13)</t>
+  </si>
+  <si>
+    <t>Cliente envia validação</t>
   </si>
 </sst>
 </file>
@@ -587,6 +587,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -596,6 +610,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -605,28 +622,11 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -914,7 +914,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,42 +923,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="21"/>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
       <c r="J2" s="1"/>
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="30"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="20" t="s">
         <v>4</v>
       </c>
@@ -986,10 +986,10 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="22">
@@ -1009,8 +1009,8 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="22">
         <v>2</v>
       </c>
@@ -1028,8 +1028,8 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="33"/>
+      <c r="B6" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="22">
@@ -1049,8 +1049,8 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="22">
         <v>4</v>
       </c>
@@ -1061,15 +1061,15 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="5"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="22">
         <v>5</v>
       </c>
@@ -1087,10 +1087,10 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="31" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="22">
@@ -1110,18 +1110,18 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="22">
         <v>7</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1129,18 +1129,18 @@
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="22">
         <v>8</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1148,16 +1148,16 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="8">
         <v>9</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="10"/>
@@ -1167,8 +1167,8 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="22">
@@ -1178,7 +1178,7 @@
         <v>19</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
@@ -1188,13 +1188,13 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="34">
+      <c r="A14" s="36"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="23">
         <v>11</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>32</v>
+      <c r="D14" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1207,22 +1207,22 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="30" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="15">
         <v>12</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17" t="s">
-        <v>15</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="17"/>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
@@ -1230,34 +1230,34 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="14">
         <v>13</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37">
+      <c r="A17" s="29"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="25">
         <v>14</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
@@ -1267,11 +1267,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B4:B5"/>
@@ -1280,6 +1275,11 @@
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.51180599999999998" right="0.51180599999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.315278" footer="0.315278"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" r:id="rId1"/>

</xml_diff>